<commit_message>
Update Servo Angles Calibration.xlsx
</commit_message>
<xml_diff>
--- a/Servo Angles Calibration.xlsx
+++ b/Servo Angles Calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mekay\Documents\GitHub\PiCar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BE7635-B664-452F-B92A-5628C4EAAE8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EA2A70-60A3-40CD-837B-64AD7EF28611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{75126306-F11D-48D3-AB71-89E58F4248F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{75126306-F11D-48D3-AB71-89E58F4248F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Calculating Servo Angles</t>
   </si>
@@ -78,34 +78,49 @@
     <t>Set 0 axis to be 90 deg on servo. Then the hip angle on left side is 360 - 341 giving u 19 deg. 19 deg subtracted from 90 gives you 71 from zero axis.   Right side: 198 - 180 , subtract that from 90 and use that on zero axis.</t>
   </si>
   <si>
-    <t>90 deg on servo angle is the axis 0 mark.0 deg is upright. 180 is down.  So 341 input should yield a 19 deg angle below the horizontal. So servo should receive angle of 109. Offset: (360 - theta1) + 90 deg</t>
-  </si>
-  <si>
     <t>Calibrating L Back Hip</t>
   </si>
   <si>
     <t>Calibrating L back knee</t>
   </si>
   <si>
-    <t xml:space="preserve">actual knee only really has a bit over 90 deg of range of motion. et servo 180 point to be when knee is all the way at the bottom, perpendicular to ground. 249 deg should yield 21 deg above this point, Offset: 180 -  (270 - theta 2)  </t>
-  </si>
-  <si>
     <t>Calibrating L Back Ankle</t>
   </si>
   <si>
-    <t>Cant do -0.22 elevationg cause of ROM concerne with ankle so im going to try using 20cm which states an angle of 67 degrees. If I set the bottoming point to be 180 deg on servo (point where ankle is max range of motion when knee is at 90deg)  then for this leg, 160 servo angle is where ankle and knee are at 90 deg, which correponds to the models theta3 = 90. So if i want a theta 3 of 67 deg. if theta 3 is less than 90, i do 160 - (90 - theta 3). if theta 3 is greater than 90 i do: 160 - theta 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test -20cm z, </t>
-  </si>
-  <si>
-    <t>339.5, 237.2, 67.2</t>
-  </si>
-  <si>
     <t>Observed Angle</t>
   </si>
   <si>
     <t>Input Angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">339.5, 234.5, 70.9 </t>
+  </si>
+  <si>
+    <t>Test -20cm z, Left Back</t>
+  </si>
+  <si>
+    <t>Ater offset</t>
+  </si>
+  <si>
+    <t>Goddamn, if max range on code is 180, but max on servo is 120 I need there to be a ratio. Y = (x/120)* 180</t>
+  </si>
+  <si>
+    <t>90 deg on servo angle is the axis 0 mark.0 deg is upright. 120 is down.  So 339 input should yield a 21 deg angle below the horizontal. So servo should receive angle of 111. Offset: (360 - theta1) + 90 deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual knee only really has a bit over 90 deg of range of motion. et servo 120 point to be when knee is all the way at the bottom, perpendicular to ground. 234 deg should yield 36 deg above this point, Offset: 120 -  (270 - theta 2)  </t>
+  </si>
+  <si>
+    <t>Cant do -0.22 elevationg cause of ROM concerne with ankle so im going to try using 20cm which states an angle of 67 degrees. If I set the bottoming point to be 120 deg on servo (point where ankle is max range of motion when knee is at 90deg)  then for this leg, 160 servo angle is where ankle and knee are at 90 deg, which correponds to the models theta3 = 90. So if i want a theta 3 of 67 deg. if theta 3 is less than 90, i do 160 - (90 - theta 3). if theta 3 is greater than 90 i do: 160 - theta 3</t>
+  </si>
+  <si>
+    <t>ankle set to 120 deg for bottomed out position at max range. Min angle is around 70deg. Models 90 deg point is 100on the servo. So if I want a theta of 71 deg.  I could do 71 + 10</t>
+  </si>
+  <si>
+    <t>the thing I need to consider is that if the knee angle changes, the ankle still maintains its angle relative to the floot, and also the range of motion changes. if I change the theta 2 angle by 70, then I need to adjust the end effector theta 3 angle by 70 just to maintain the position. so i coul dsay when the model tells theta 2 to change by an angle, i add that offset to theta 3. theta 2- theta2 '  offet to 3? might be a more elgean tway to implemetn this tho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want the middle of the mechanical range and the middle of the servo range to line up. </t>
   </si>
 </sst>
 </file>
@@ -483,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5120EF2E-58D2-406D-A14B-E1A354954992}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,21 +510,27 @@
     <col min="2" max="2" width="33.77734375" customWidth="1"/>
     <col min="3" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="4" width="30.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="5" max="5" width="39.21875" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
     <col min="7" max="7" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -526,10 +547,10 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -543,7 +564,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -557,7 +578,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -571,7 +592,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -585,12 +606,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -598,7 +619,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="171.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="171.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -607,28 +628,40 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="22" spans="1:2" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="216.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="216.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="224.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="224.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -640,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70958A77-C015-4636-885A-CCFD66A5B7F0}">
   <dimension ref="A3:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -652,10 +685,10 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>